<commit_message>
sync and integrate with ControlWorksAnalyzer
</commit_message>
<xml_diff>
--- a/docs/GradeReport.xlsx
+++ b/docs/GradeReport.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>Матем</t>
   </si>
@@ -209,9 +209,6 @@
     <t>В один ряд</t>
   </si>
   <si>
-    <t>Итоговая</t>
-  </si>
-  <si>
     <t>Прикреплена к периоду по индексу</t>
   </si>
   <si>
@@ -224,9 +221,6 @@
     <t>Выбранный предмет</t>
   </si>
   <si>
-    <t>Расчитать итоговую</t>
-  </si>
-  <si>
     <t>Одинакова среди семестров данного предмета</t>
   </si>
   <si>
@@ -245,15 +239,6 @@
     <t>Одинаковы на период обучения</t>
   </si>
   <si>
-    <t>Период 1</t>
-  </si>
-  <si>
-    <t>Период 2</t>
-  </si>
-  <si>
-    <t>Период 3</t>
-  </si>
-  <si>
     <t>Корневич Максим</t>
   </si>
   <si>
@@ -266,59 +251,29 @@
     <t>Предмет 2</t>
   </si>
   <si>
-    <t>Следующий учащийся</t>
-  </si>
-  <si>
-    <t>Здвиг каретки вправо</t>
-  </si>
-  <si>
-    <t>После ввода оценки</t>
-  </si>
-  <si>
-    <t>* - 10</t>
-  </si>
-  <si>
-    <t>Ничего не делать</t>
-  </si>
-  <si>
-    <t>Режим</t>
-  </si>
-  <si>
-    <t>Изменить</t>
-  </si>
-  <si>
-    <t>Добавить слева</t>
-  </si>
-  <si>
-    <t>№</t>
-  </si>
-  <si>
-    <t>Расчитать семестровую</t>
-  </si>
-  <si>
-    <t>ESC - Предыдущий учащийся</t>
-  </si>
-  <si>
-    <t>Enter - Следующий учучащийся</t>
-  </si>
-  <si>
     <t>Козляковский Илья</t>
   </si>
   <si>
-    <t>Опорный период</t>
-  </si>
-  <si>
-    <t>Период ячейки</t>
-  </si>
-  <si>
-    <t>Семестр ячейки</t>
+    <t>СЕМ</t>
+  </si>
+  <si>
+    <t>КУР</t>
+  </si>
+  <si>
+    <t>ЭКЗ</t>
+  </si>
+  <si>
+    <t>Добавить курсовую</t>
+  </si>
+  <si>
+    <t>Добавить экзаменационную</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -350,6 +305,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -359,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -382,74 +360,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -472,25 +387,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1071,7 +1013,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,13 +1027,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1108,13 +1050,13 @@
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1131,13 +1073,13 @@
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1154,13 +1096,13 @@
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1177,13 +1119,13 @@
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1200,13 +1142,13 @@
       <c r="A6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1221,9 +1163,9 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -1232,13 +1174,13 @@
       <c r="A8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1251,40 +1193,101 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+    </row>
     <row r="11" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="13" t="s">
         <v>69</v>
       </c>
+      <c r="C11" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="E11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="G11" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="12" t="s">
         <v>59</v>
       </c>
       <c r="E23" t="s">
@@ -1299,15 +1302,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,293 +1319,551 @@
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" customWidth="1"/>
     <col min="3" max="3" width="3.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="16" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" customWidth="1"/>
+    <col min="8" max="16" width="3.7109375" customWidth="1"/>
     <col min="18" max="18" width="36.140625" customWidth="1"/>
     <col min="19" max="19" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="9">
+        <v>8</v>
+      </c>
+      <c r="F2" s="9">
+        <v>7</v>
+      </c>
+      <c r="G2" s="28">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="12">
-        <v>1</v>
-      </c>
-      <c r="H1" s="12">
+      <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="I1" s="12">
+      <c r="D3" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="9">
+        <v>8</v>
+      </c>
+      <c r="F3" s="29">
+        <v>8</v>
+      </c>
+      <c r="G3" s="9">
+        <v>7</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="9">
         <v>3</v>
       </c>
-      <c r="J1" s="12">
-        <v>4</v>
-      </c>
-      <c r="K1" s="12">
-        <v>5</v>
-      </c>
-      <c r="L1" s="12">
-        <v>6</v>
-      </c>
-      <c r="M1" s="12">
+      <c r="D4" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="9">
         <v>7</v>
       </c>
-      <c r="N1" s="12">
+      <c r="F4" s="9">
         <v>8</v>
       </c>
-      <c r="O1" s="12">
-        <v>9</v>
-      </c>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
-      <c r="R2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="14">
-        <v>1</v>
-      </c>
-      <c r="H3" s="14">
-        <v>3</v>
-      </c>
-      <c r="I3" s="14">
-        <v>6</v>
-      </c>
-      <c r="J3" s="14">
+      <c r="G4" s="9">
         <v>8</v>
       </c>
-      <c r="K3" s="14">
-        <v>9</v>
-      </c>
-      <c r="L3" s="14">
-        <v>6</v>
-      </c>
-      <c r="M3" s="14">
-        <v>7</v>
-      </c>
-      <c r="N3" s="14">
-        <v>8</v>
-      </c>
-      <c r="O3" s="14">
-        <v>3</v>
-      </c>
-      <c r="P3" s="14"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9">
-        <v>5</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="R4" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="R5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="R6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="R9" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>74</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>94</v>
-      </c>
-      <c r="R12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R15" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>88</v>
-      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="18"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="18"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+      <c r="S14" s="18"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="18"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="18"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+      <c r="S17" s="18"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+      <c r="S18" s="18"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="25"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="18"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add grade type, special grades
</commit_message>
<xml_diff>
--- a/docs/GradeReport.xlsx
+++ b/docs/GradeReport.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="3"/>
+    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="6" r:id="rId1"/>
     <sheet name="Лист1" sheetId="8" r:id="rId2"/>
     <sheet name="Типы оценок" sheetId="7" r:id="rId3"/>
     <sheet name="Лист3" sheetId="10" r:id="rId4"/>
+    <sheet name="Лист2" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
   <si>
     <t>Матем</t>
   </si>
@@ -267,13 +268,34 @@
   </si>
   <si>
     <t>Добавить экзаменационную</t>
+  </si>
+  <si>
+    <t>Типы оценок</t>
+  </si>
+  <si>
+    <t>Курсовая(0)</t>
+  </si>
+  <si>
+    <t>Экзаменационная (0)</t>
+  </si>
+  <si>
+    <t>Семестровая (0)</t>
+  </si>
+  <si>
+    <t>Позиция 1 [&lt;] [&gt;] [+] [-]</t>
+  </si>
+  <si>
+    <t>Сохранить</t>
+  </si>
+  <si>
+    <t>Доступно Осв/Зач</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,6 +350,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -364,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -434,6 +477,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1010,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1248,39 +1302,45 @@
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>58</v>
       </c>
@@ -1310,8 +1370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1869,4 +1929,593 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" customWidth="1"/>
+    <col min="8" max="16" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="36.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="9">
+        <v>1</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="9">
+        <v>8</v>
+      </c>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="R1" s="34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="9">
+        <v>8</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="9">
+        <v>7</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="14"/>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="36"/>
+      <c r="S7" s="18"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="18"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="18"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="18"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="S11" s="18"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="S12" s="18"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="S13" s="18"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="S14" s="18"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="18"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="18"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="18"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="18"/>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="18"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="18"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="18"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="18"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="18"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="34"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="18"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="34"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="18"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
+      <c r="R25" s="37"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="R26" s="37"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="33"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
design grade editor form
</commit_message>
<xml_diff>
--- a/docs/GradeReport.xlsx
+++ b/docs/GradeReport.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="89">
   <si>
     <t>Матем</t>
   </si>
@@ -289,6 +289,12 @@
   </si>
   <si>
     <t>Доступно Осв/Зач</t>
+  </si>
+  <si>
+    <t>Если нету то не отображать столбец с оценками</t>
+  </si>
+  <si>
+    <t>Сохраняет оценки глобально для семестра</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1942,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1956,7 @@
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="16" width="3.7109375" customWidth="1"/>
     <col min="18" max="18" width="36.140625" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="19" max="19" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2010,7 +2016,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>
@@ -2039,8 +2045,8 @@
       <c r="S3" s="14"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
+      <c r="A4" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -2060,8 +2066,8 @@
       <c r="S4" s="14"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>72</v>
+      <c r="A5" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="16"/>
@@ -2079,9 +2085,6 @@
       <c r="S5" s="14"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>73</v>
-      </c>
       <c r="E6" s="14"/>
       <c r="F6" s="16"/>
       <c r="G6" s="15"/>
@@ -2186,7 +2189,9 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="D11" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
@@ -2203,7 +2208,9 @@
       <c r="R11" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="S11" s="18"/>
+      <c r="S11" s="18" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>

</xml_diff>

<commit_message>
start develop grade editor
</commit_message>
<xml_diff>
--- a/docs/GradeReport.xlsx
+++ b/docs/GradeReport.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="4"/>
+    <workbookView xWindow="6480" yWindow="3945" windowWidth="27555" windowHeight="14745" tabRatio="815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="6" r:id="rId1"/>
@@ -1376,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>

</xml_diff>